<commit_message>
Add in current spawners to diagnostic scenarios tab, remove current and historical scenarios from scenario column
</commit_message>
<xml_diff>
--- a/srt_figures/spawners_template.xlsx
+++ b/srt_figures/spawners_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Species</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Spawners</t>
+  </si>
+  <si>
+    <t>Spawners Current Scenario</t>
   </si>
 </sst>
 </file>
@@ -503,18 +506,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="30.7109375" customWidth="1"/>
+    <col min="1" max="10" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,15 +534,18 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Pn to spawners_workbook.xlxs
* Merge spawners_subbasin.R and spawners_diagnostic_scenarios.R
* Minor cleanup
</commit_message>
<xml_diff>
--- a/srt_figures/spawners_template.xlsx
+++ b/srt_figures/spawners_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Projects\Chehalis\ASRP\asrp_git\srt_figures\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EDR Spawners" sheetId="6" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Subbasin Spawners" sheetId="7" r:id="rId3"/>
     <sheet name="Subbasin Diagnostic Scenarios" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
   <si>
     <t>Species</t>
   </si>
@@ -68,12 +73,18 @@
   </si>
   <si>
     <t>Diagnostic scenario</t>
+  </si>
+  <si>
+    <t>Rank (Pn change)</t>
+  </si>
+  <si>
+    <t>Productivity (Pn) change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,6 +177,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -213,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,7 +262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,10 +482,12 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="16" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="16" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,6 +520,12 @@
       </c>
       <c r="K1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -514,10 +536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,10 +548,12 @@
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" style="4" customWidth="1"/>
-    <col min="13" max="16" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -565,6 +589,12 @@
       </c>
       <c r="L1" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -576,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,8 +659,12 @@
       <c r="M1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="N1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -645,10 +679,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,10 +692,10 @@
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="14" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -703,6 +737,12 @@
       </c>
       <c r="N1" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add in ASRP tabs and outputs from V13.1 with Hist 2040 and Hist 2080
</commit_message>
<xml_diff>
--- a/srt_figures/spawners_template.xlsx
+++ b/srt_figures/spawners_template.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="7755" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EDR Spawners" sheetId="6" r:id="rId1"/>
     <sheet name="EDR Diagnostic Scenarios" sheetId="9" r:id="rId2"/>
-    <sheet name="Subbasin Spawners" sheetId="7" r:id="rId3"/>
-    <sheet name="Subbasin Diagnostic Scenarios" sheetId="8" r:id="rId4"/>
+    <sheet name="EDR ASRP Scenarios" sheetId="10" r:id="rId3"/>
+    <sheet name="Subbasin Spawners" sheetId="7" r:id="rId4"/>
+    <sheet name="Subbasin Diagnostic Scenarios" sheetId="8" r:id="rId5"/>
+    <sheet name="Subbasin ASRP Scenarios" sheetId="11" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="19">
   <si>
     <t>Species</t>
   </si>
@@ -538,7 +540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -604,6 +606,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="4" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -619,7 +689,7 @@
     <col min="5" max="21" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -677,7 +747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
@@ -695,7 +765,7 @@
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -736,6 +806,81 @@
         <v>10</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
+    <col min="5" max="14" width="15.7109375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="O1" s="7" t="s">

</xml_diff>

<commit_message>
Add script to make 3 GSU level plots, add code to make ASRP spawner change plots, updates to spawner table
* Adjust spawner table code so it is not reliant on running the full model
* Separate year (climate) from ASRP names and fix scenario names
* Remove 'Unnamed :' from subbasins
* Add colors to spawner_template.xlxs
</commit_message>
<xml_diff>
--- a/srt_figures/spawners_template.xlsx
+++ b/srt_figures/spawners_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="7755" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EDR Spawners" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
   <si>
     <t>Species</t>
   </si>
@@ -68,12 +68,6 @@
     <t>Scenario</t>
   </si>
   <si>
-    <t>Diagnostic scenario spawners</t>
-  </si>
-  <si>
-    <t>Rank(percent change)</t>
-  </si>
-  <si>
     <t>Diagnostic scenario</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>Productivity (Pn) change</t>
+  </si>
+  <si>
+    <t>Diagnosic scenario</t>
+  </si>
+  <si>
+    <t>Climate</t>
   </si>
 </sst>
 </file>
@@ -107,7 +107,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +117,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,25 +178,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -475,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,44 +526,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -540,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,35 +585,35 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="17.140625" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" customWidth="1"/>
     <col min="15" max="16" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -586,17 +622,17 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -606,65 +642,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
-    <col min="3" max="12" width="15.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="4" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="2" customWidth="1"/>
+    <col min="15" max="16" width="30.7109375" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>17</v>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -674,10 +719,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,61 +731,55 @@
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="21" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -751,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,54 +804,54 @@
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -823,71 +862,76 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
-    <col min="5" max="14" width="15.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="5" max="14" width="15.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update code to create_spawner_tbl and code to create GSU figs
* Have the GSU fig script source data from the passage_sed_bip.R and the Excel sheet
* Tweak passage_sed_bip.R so it runs smooth
* Complete overhaul of create_spawner_tbl so reduce redundancy between EDR and subbasin scale analysis
* Tweak the spawner_tbl template
</commit_message>
<xml_diff>
--- a/srt_figures/spawners_template.xlsx
+++ b/srt_figures/spawners_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Species</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>Climate</t>
+  </si>
+  <si>
+    <t>Diagnostic scenario spawners</t>
+  </si>
+  <si>
+    <t>Spawner change (per km)</t>
+  </si>
+  <si>
+    <t>Blah blah</t>
   </si>
 </sst>
 </file>
@@ -178,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -203,6 +212,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,7 +540,7 @@
     <col min="14" max="16" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -642,10 +657,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,60 +670,54 @@
     <col min="3" max="12" width="15.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="17.140625" style="2" customWidth="1"/>
     <col min="14" max="14" width="13.5703125" style="2" customWidth="1"/>
-    <col min="15" max="16" width="30.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="15" max="15" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H1" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="N1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="O1" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -734,7 +743,7 @@
     <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -804,7 +813,7 @@
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -881,7 +890,7 @@
     <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="9" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>

</xml_diff>